<commit_message>
check suppl. images for AT
</commit_message>
<xml_diff>
--- a/Plancheck/plancheck_data/check_protocol/STEC vertebre L5-3F.xlsx
+++ b/Plancheck/plancheck_data/check_protocol/STEC vertebre L5-3F.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="207">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -629,6 +629,21 @@
   </si>
   <si>
     <t>D0,5cc&lt;33Gy</t>
+  </si>
+  <si>
+    <t>Suppl. Image3D nécessaires</t>
+  </si>
+  <si>
+    <t>Chaque élement séparé par ** doit être dans le nom de la série</t>
+  </si>
+  <si>
+    <t>T1**SPACE**3D</t>
+  </si>
+  <si>
+    <t>T2**SPACE**3D</t>
+  </si>
+  <si>
+    <t>T1**GADO**DIXON</t>
   </si>
 </sst>
 </file>
@@ -1192,7 +1207,7 @@
     <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1286,6 +1301,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1614,8 +1635,8 @@
   </sheetPr>
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,9 +2366,31 @@
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
+        <v>202</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="L52" s="15" t="s">
         <v>65</v>
       </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="B53" s="35" t="s">
+        <v>205</v>
+      </c>
+      <c r="C53" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="30"/>
+      <c r="H53" s="30"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L55" s="15" t="s">
@@ -2878,7 +2921,7 @@
   </sheetPr>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D32"/>
     </sheetView>
   </sheetViews>

</xml_diff>